<commit_message>
importacion de datetime y creacion de los metodos reserva de servicios
</commit_message>
<xml_diff>
--- a/DATA/datos.xlsx
+++ b/DATA/datos.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Servicios" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Contraseñas" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Inventario" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="ReservasServicios" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -752,4 +753,80 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="9" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID Reserva</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Servicio</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha Reserva</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha Servicio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>mgiue</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>345</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>28/05/2024 14:25</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>28/05/2024 14:30</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>